<commit_message>
Fix activity log export some Activity data is not shown
</commit_message>
<xml_diff>
--- a/storage/templates/activity-log.xlsx
+++ b/storage/templates/activity-log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/code/cost-control/storage/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7E5F08-9F79-3141-A088-CD2F3016BB0F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B774747-9B50-0F43-AEC4-47AAF0B3907B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driving " sheetId="3" r:id="rId1"/>
@@ -468,7 +468,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -492,27 +492,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="40" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -561,6 +545,10 @@
     <xf numFmtId="40" fontId="6" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -852,7 +840,7 @@
   <dimension ref="B1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -897,10 +885,10 @@
       </c>
       <c r="N2" s="42"/>
       <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="44"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="61"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
@@ -918,15 +906,15 @@
       <c r="J3" s="33"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="45" t="s">
+      <c r="M3" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="47"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="63"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
@@ -1060,12 +1048,12 @@
     <mergeCell ref="I6:S6"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="R2:S2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="H3:J3"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="P3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1107,64 +1095,64 @@
       <c r="B2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
-      <c r="M2" s="61" t="s">
+      <c r="M2" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="58"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="22"/>
       <c r="L3" s="22"/>
-      <c r="M3" s="62" t="s">
+      <c r="M3" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="60"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="56"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
@@ -1192,26 +1180,26 @@
       <c r="Q5" s="26"/>
     </row>
     <row r="6" spans="2:17" ht="23" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53" t="s">
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="55"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="51"/>
     </row>
     <row r="7" spans="2:17" s="31" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="27" t="s">

</xml_diff>